<commit_message>
Debug de Decoder a Pasos
</commit_message>
<xml_diff>
--- a/archivoPatron.xlsx
+++ b/archivoPatron.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estudianteccr-my.sharepoint.com/personal/alexsq_estudiantec_cr/Documents/Semestre 2-2023/Micros/ProyectoGrua/Proyecto_Grua_Micros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_AD4D2F04E46CFB4ACB3E20395517DACE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D62AA1CD-5EC2-49B3-A398-41EB809A0918}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="11_AD4D2F04E46CFB4ACB3E20395517DACE693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA52EE2-1956-410F-A189-98473961B784}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +70,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -218,39 +230,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +563,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,73 +572,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="5">
         <v>100</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>200</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="6">
         <v>300</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="16">
         <v>100</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="2">
         <v>200</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="15">
         <v>300</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="16">
         <v>100</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <v>200</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="15">
         <v>300</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>